<commit_message>
Modifying database migrations to match the database mapping
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C81879D-C636-490B-9994-DC32127D27A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE0E124-739E-4F37-83B3-B001BB145B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>user</t>
   </si>
@@ -49,9 +49,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>date_of_birth</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>avatar_image</t>
-  </si>
-  <si>
     <t>Foreign key</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>manager_id</t>
   </si>
   <si>
-    <t>session_id</t>
-  </si>
-  <si>
     <t>coach_id</t>
   </si>
   <si>
@@ -133,22 +124,43 @@
     <t>Composite</t>
   </si>
   <si>
-    <t>attendance</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>attendace_datetime</t>
-  </si>
-  <si>
     <t>purchases</t>
   </si>
   <si>
-    <t>package_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">We Have to specify the gym_id because we The requirnents said that we need to know from which gym the package bought so the manager her could be (gymManager or admin or city_manager) so we have to store the gym id her </t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>email_verified_at</t>
+  </si>
+  <si>
+    <t>is_banned</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>coaches_table</t>
+  </si>
+  <si>
+    <t>training_session_id</t>
+  </si>
+  <si>
+    <t>attendances</t>
+  </si>
+  <si>
+    <t>attendance_datetime</t>
+  </si>
+  <si>
+    <t>training_package_id</t>
   </si>
 </sst>
 </file>
@@ -724,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
-  <dimension ref="A2:K35"/>
+  <dimension ref="A2:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30:J35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -737,29 +749,28 @@
     <col min="3" max="3" width="18.6640625" style="1"/>
     <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.88671875" style="1" customWidth="1"/>
-    <col min="6" max="11" width="18.6640625" style="1"/>
-    <col min="12" max="12" width="26.21875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="18.6640625" style="1"/>
+    <col min="10" max="10" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1"/>
+    <col min="12" max="12" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="18.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -770,8 +781,10 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -780,291 +793,362 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="G9" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+    </row>
+    <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>5</v>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="H14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="I14" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="17" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="D17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="15"/>
+    <row r="18" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="I19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="L19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="14"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="H20" s="8" t="s">
+      <c r="G20" s="15"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="13"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="K24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="9"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+      <c r="L27" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="H29" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+    </row>
+    <row r="30" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="F25" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="2:10" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="I32" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-    </row>
-    <row r="31" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-    </row>
-    <row r="32" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-    </row>
-    <row r="34" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
+      <c r="J32" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="35" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>30</v>
+      </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
     </row>
+    <row r="36" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F30:J35"/>
-    <mergeCell ref="B9:D10"/>
-    <mergeCell ref="B20:F21"/>
-    <mergeCell ref="B14:F15"/>
-    <mergeCell ref="H20:J21"/>
-    <mergeCell ref="B25:D26"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="C4:J5"/>
-    <mergeCell ref="I14:J15"/>
-    <mergeCell ref="G9:K10"/>
+  <mergeCells count="12">
+    <mergeCell ref="F35:J40"/>
+    <mergeCell ref="C4:L5"/>
+    <mergeCell ref="C9:J10"/>
+    <mergeCell ref="I19:J20"/>
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="C24:G25"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="H29:L30"/>
+    <mergeCell ref="L19:M20"/>
+    <mergeCell ref="H14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modifying whole database ERD, Database Seeds and factories and resources
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4ADEEB-F178-4BD3-8B71-BB3C60757B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018A38D-5049-4C47-839D-54C35EF6CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>user</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Foreign key</t>
   </si>
   <si>
-    <t>gym_manager_id</t>
-  </si>
-  <si>
     <t>gym_id</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>purchases</t>
   </si>
   <si>
-    <t xml:space="preserve">We Have to specify the gym_id because we The requirnents said that we need to know from which gym the package bought so the manager her could be (gymManager or admin or city_manager) so we have to store the gym id her </t>
-  </si>
-  <si>
     <t>birth_date</t>
   </si>
   <si>
@@ -139,12 +133,6 @@
     <t>avatar</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>client_id</t>
-  </si>
-  <si>
     <t>coaches_table</t>
   </si>
   <si>
@@ -158,13 +146,22 @@
   </si>
   <si>
     <t>training_package_id</t>
+  </si>
+  <si>
+    <t>admins</t>
+  </si>
+  <si>
+    <t>managers</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,14 +224,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -262,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -356,11 +345,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,9 +387,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,6 +412,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
-  <dimension ref="A2:M40"/>
+  <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -761,37 +762,37 @@
     </row>
     <row r="3" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
@@ -810,42 +811,42 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="C9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -861,44 +862,44 @@
         <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="13"/>
-      <c r="H14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="12"/>
+      <c r="H14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="14"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="15"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="17" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="13"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="14"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="17" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
@@ -906,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>1</v>
@@ -915,46 +916,46 @@
         <v>4</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="2" t="s">
+    </row>
+    <row r="18" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="I19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="L19" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="I19" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="L19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-    </row>
-    <row r="21" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
@@ -962,13 +963,13 @@
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>1</v>
@@ -977,39 +978,45 @@
         <v>4</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="K24" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="13"/>
-    </row>
-    <row r="25" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="J24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="N24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="15"/>
+      <c r="P24" s="12"/>
+    </row>
+    <row r="25" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
@@ -1017,131 +1024,92 @@
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="M27" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="H29" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-    </row>
-    <row r="30" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-    </row>
-    <row r="31" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J27" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="20"/>
+      <c r="N27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="H29" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+    </row>
+    <row r="31" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="6:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F35:J40"/>
+  <mergeCells count="13">
+    <mergeCell ref="J24:K25"/>
+    <mergeCell ref="J27:K27"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
     <mergeCell ref="I19:J20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
     <mergeCell ref="C19:G20"/>
-    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="N24:P25"/>
     <mergeCell ref="C29:E30"/>
     <mergeCell ref="H29:L30"/>
     <mergeCell ref="L19:M20"/>

</xml_diff>

<commit_message>
adding gym id to coach table
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6018A38D-5049-4C47-839D-54C35EF6CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAE6A40-9C5C-4AE5-889D-79705199C8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>user</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>training_package_id</t>
-  </si>
-  <si>
-    <t>admins</t>
   </si>
   <si>
     <t>managers</t>
@@ -251,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -345,20 +342,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,12 +400,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
   <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -770,7 +752,7 @@
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -934,14 +916,14 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
-      <c r="I19" s="11" t="s">
+      <c r="J19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="L19" s="10" t="s">
+      <c r="K19" s="12"/>
+      <c r="M19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="17"/>
@@ -949,10 +931,10 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
-      <c r="L20" s="10"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="14"/>
       <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -977,10 +959,13 @@
       <c r="J22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="K22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="N22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -993,10 +978,6 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
-      <c r="J24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="10"/>
       <c r="N24" s="11" t="s">
         <v>22</v>
       </c>
@@ -1009,8 +990,6 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
       <c r="N25" s="13"/>
       <c r="O25" s="16"/>
       <c r="P25" s="14"/>
@@ -1032,10 +1011,6 @@
       <c r="G27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" s="20"/>
       <c r="N27" s="8" t="s">
         <v>24</v>
       </c>
@@ -1075,7 +1050,7 @@
     </row>
     <row r="32" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>33</v>
@@ -1087,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J32" s="7" t="s">
         <v>36</v>
@@ -1100,20 +1075,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="J24:K25"/>
-    <mergeCell ref="J27:K27"/>
+  <mergeCells count="11">
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="H29:L30"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="H14:L15"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
-    <mergeCell ref="I19:J20"/>
+    <mergeCell ref="J19:K20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
     <mergeCell ref="C19:G20"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="H29:L30"/>
-    <mergeCell ref="L19:M20"/>
-    <mergeCell ref="H14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modifying the side bar to be flexible acording to the loged in user permissions
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAE6A40-9C5C-4AE5-889D-79705199C8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F676DD58-F819-4430-B5EC-C07DB236E307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
@@ -375,31 +375,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
   <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -751,30 +751,30 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
@@ -809,26 +809,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -858,28 +858,28 @@
     </row>
     <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="17" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
@@ -909,32 +909,32 @@
     </row>
     <row r="18" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="11" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="J19" s="10" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="12"/>
-      <c r="M19" s="10" t="s">
+      <c r="M19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N19" s="10"/>
+      <c r="N19" s="18"/>
     </row>
     <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
       <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="K20" s="15"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
     </row>
     <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -971,28 +971,28 @@
     </row>
     <row r="23" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="N24" s="11" t="s">
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="N24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="15"/>
+      <c r="O24" s="11"/>
       <c r="P24" s="12"/>
     </row>
     <row r="25" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
       <c r="N25" s="13"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="15"/>
     </row>
     <row r="26" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1022,28 +1022,28 @@
       </c>
     </row>
     <row r="29" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="H29" s="17" t="s">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="H29" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
     </row>
     <row r="31" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K31" s="9"/>
@@ -1076,17 +1076,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="H29:L30"/>
-    <mergeCell ref="M19:N20"/>
-    <mergeCell ref="H14:L15"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
     <mergeCell ref="J19:K20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
     <mergeCell ref="C19:G20"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="H29:L30"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="H14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modifying Attendacnes and Purchases return data to return only the required and finishing gym Manager
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7A6FE4-58FA-4A7B-8ECB-7E1029E5C6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB6F7F1-8FCD-49FD-A3AB-1CF14108EB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
@@ -375,31 +375,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
   <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -751,30 +751,30 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
@@ -809,26 +809,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -858,28 +858,28 @@
     </row>
     <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="17" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
@@ -909,32 +909,32 @@
     </row>
     <row r="18" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="11" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="J19" s="10" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="12"/>
-      <c r="M19" s="10" t="s">
+      <c r="M19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N19" s="10"/>
+      <c r="N19" s="18"/>
     </row>
     <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
       <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="K20" s="15"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
     </row>
     <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -971,28 +971,28 @@
     </row>
     <row r="23" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="N24" s="11" t="s">
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="N24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="15"/>
+      <c r="O24" s="11"/>
       <c r="P24" s="12"/>
     </row>
     <row r="25" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
       <c r="N25" s="13"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="15"/>
     </row>
     <row r="26" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1022,28 +1022,28 @@
       </c>
     </row>
     <row r="29" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="H29" s="17" t="s">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="H29" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
     </row>
     <row r="31" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K31" s="9"/>
@@ -1076,17 +1076,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="H29:L30"/>
-    <mergeCell ref="M19:N20"/>
-    <mergeCell ref="H14:L15"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
     <mergeCell ref="J19:K20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
     <mergeCell ref="C19:G20"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="H29:L30"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="H14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finishing General Managers Datatables and adding General Managers Seeders
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB6F7F1-8FCD-49FD-A3AB-1CF14108EB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30873BD2-D769-47EC-9A48-6174A18157C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,31 +375,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
   <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -751,30 +751,30 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
@@ -809,26 +809,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -858,28 +858,28 @@
     </row>
     <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="12"/>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="14"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="17" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
@@ -909,32 +909,32 @@
     </row>
     <row r="18" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="J19" s="10" t="s">
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="J19" s="11" t="s">
         <v>32</v>
       </c>
       <c r="K19" s="12"/>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N19" s="18"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="J20" s="13"/>
-      <c r="K20" s="15"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
+      <c r="K20" s="14"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -971,28 +971,28 @@
     </row>
     <row r="23" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="N24" s="10" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="N24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="11"/>
+      <c r="O24" s="15"/>
       <c r="P24" s="12"/>
     </row>
     <row r="25" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
       <c r="N25" s="13"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="15"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="14"/>
     </row>
     <row r="26" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1022,28 +1022,28 @@
       </c>
     </row>
     <row r="29" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="H29" s="16" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="H29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K31" s="9"/>
@@ -1076,17 +1076,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="H29:L30"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="H14:L15"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
     <mergeCell ref="J19:K20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
     <mergeCell ref="C19:G20"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="H29:L30"/>
-    <mergeCell ref="M19:N20"/>
-    <mergeCell ref="H14:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding creator relation to the gym
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30873BD2-D769-47EC-9A48-6174A18157C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2051326-C54D-414B-8FF4-E43ADD210E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>user</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>creator_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -375,31 +381,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
-  <dimension ref="A2:P32"/>
+  <dimension ref="A2:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -731,8 +737,8 @@
     <col min="5" max="5" width="25.88671875" style="1" customWidth="1"/>
     <col min="6" max="9" width="18.6640625" style="1"/>
     <col min="10" max="10" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1"/>
-    <col min="12" max="12" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.21875" style="1" customWidth="1"/>
     <col min="13" max="16384" width="18.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -751,30 +757,30 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
@@ -809,26 +815,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -858,30 +864,32 @@
     </row>
     <row r="13" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="14"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="17" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+    </row>
+    <row r="17" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
@@ -891,14 +899,17 @@
       <c r="E17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>13</v>
@@ -907,95 +918,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="17" t="s">
-        <v>18</v>
+    <row r="18" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="11" t="s">
+      <c r="F19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="M19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="J19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="18"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
       <c r="J20" s="13"/>
       <c r="K20" s="14"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="3" t="s">
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="J22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="17" t="s">
+    </row>
+    <row r="24" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="N24" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O24" s="15"/>
-      <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="14"/>
-    </row>
-    <row r="26" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="J24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+    </row>
+    <row r="25" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+    </row>
+    <row r="26" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
@@ -1011,82 +1013,97 @@
       <c r="G27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O27" s="8" t="s">
+      <c r="J27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="P27" s="7" t="s">
+      <c r="L27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+    </row>
+    <row r="31" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="H29" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="3:16" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="3:16" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="7" t="s">
+      <c r="M32" s="7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I34" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="H29:L30"/>
-    <mergeCell ref="M19:N20"/>
-    <mergeCell ref="H14:L15"/>
     <mergeCell ref="C4:L5"/>
     <mergeCell ref="C9:J10"/>
-    <mergeCell ref="J19:K20"/>
     <mergeCell ref="C14:E15"/>
     <mergeCell ref="C24:G25"/>
-    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="C29:G30"/>
+    <mergeCell ref="F19:H20"/>
+    <mergeCell ref="G14:L15"/>
+    <mergeCell ref="J19:L20"/>
+    <mergeCell ref="J24:L25"/>
+    <mergeCell ref="I29:M30"/>
+    <mergeCell ref="C19:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding packages method in the user that define the many to many relation
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12DBDD8-5E83-4B2D-8D6E-E9886FE08AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80486DAE-8BF6-4949-81BA-4B028C4A62ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
   <dimension ref="A2:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding amount_paid, sessions_number to purchases table
</commit_message>
<xml_diff>
--- a/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
+++ b/00 Project Material/01 Database/00 ERD/ERD Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03 Work\05 Programming\00 Git Hub Repos\00 ITI\05 simple_gym_app\00 Project Material\01 Database\00 ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80486DAE-8BF6-4949-81BA-4B028C4A62ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23939B7-76B5-4C72-B511-0626B617C847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2CCCDF1-FECE-4E37-A74D-A57AB737D47D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>user</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>amount_paid</t>
   </si>
 </sst>
 </file>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3846C555-CB77-4716-A2C3-7FE0759C5F04}">
-  <dimension ref="A2:M34"/>
+  <dimension ref="A2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="H23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -889,7 +892,7 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="17" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
@@ -918,8 +921,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="10" t="s">
         <v>11</v>
       </c>
@@ -935,7 +938,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="F20" s="17"/>
@@ -945,8 +948,8 @@
       <c r="K20" s="15"/>
       <c r="L20" s="16"/>
     </row>
-    <row r="21" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -972,7 +975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="17" t="s">
         <v>15</v>
       </c>
@@ -986,7 +989,7 @@
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
-    <row r="25" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -996,8 +999,8 @@
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
-    <row r="26" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="17" t="s">
         <v>18</v>
       </c>
@@ -1038,8 +1041,10 @@
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
-    </row>
-    <row r="30" spans="3:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+    </row>
+    <row r="30" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -1050,11 +1055,13 @@
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
-    </row>
-    <row r="31" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+    </row>
+    <row r="31" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L31" s="9"/>
     </row>
-    <row r="32" spans="3:13" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
@@ -1084,6 +1091,12 @@
       </c>
       <c r="M32" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="9:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1102,8 +1115,8 @@
     <mergeCell ref="G14:L15"/>
     <mergeCell ref="J19:L20"/>
     <mergeCell ref="J24:L25"/>
-    <mergeCell ref="I29:M30"/>
     <mergeCell ref="C19:D20"/>
+    <mergeCell ref="I29:O30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>